<commit_message>
find user by name then find their id
</commit_message>
<xml_diff>
--- a/webroot/uploads/user_payroll_details.xlsx
+++ b/webroot/uploads/user_payroll_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A03AB1-517F-4937-928D-3ED38A6C26A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824DE70C-AC96-48FF-B36B-A688B5B81249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{111B8372-6BEE-48AE-9B8E-2909592D2964}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Basic Salary</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Risk Allowance</t>
+  </si>
+  <si>
+    <t>Elijah Kyule</t>
+  </si>
+  <si>
+    <t>Christopher Ndemi</t>
+  </si>
+  <si>
+    <t>Tobias Mwalili</t>
   </si>
 </sst>
 </file>
@@ -402,12 +411,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
@@ -428,7 +437,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2">
@@ -442,7 +451,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
@@ -456,17 +465,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="C4" s="1">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D4">
-        <v>6000</v>
+        <v>9000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>